<commit_message>
Validacion examen Roque Estructura de Datos Dual
</commit_message>
<xml_diff>
--- a/CLAVES_VALIDACIÓN_EXAMEN.xlsx
+++ b/CLAVES_VALIDACIÓN_EXAMEN.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mkey\utags\2019\Septiembre_Diciembre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkey\Desktop\Septiembre_Diciembre\Septiembre_Diciembre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC8A511-DB32-46E0-8FE1-B13AF4FF7EA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{70B3D11C-390F-416B-BEA9-C5F86ECB31AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>DíaEntregado</t>
   </si>
@@ -230,12 +229,21 @@
   </si>
   <si>
     <t>30OCT</t>
+  </si>
+  <si>
+    <t>01NOV</t>
+  </si>
+  <si>
+    <t>RRC</t>
+  </si>
+  <si>
+    <t>04D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -589,7 +597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5C6488-4A61-4D63-9777-F049B3AE8F94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:H2"/>
   <sheetViews>
@@ -643,12 +651,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2CFC11-BD85-4A01-9BD4-099AFE1156B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +984,7 @@
         <v>23</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I21" si="1">CONCATENATE(B13,C13,D13,E13,F13,G13,H13)</f>
+        <f t="shared" ref="I13:I22" si="1">CONCATENATE(B13,C13,D13,E13,F13,G13,H13)</f>
         <v>07OCTMP0201GCAMARRL_00001</v>
       </c>
     </row>
@@ -1194,6 +1202,33 @@
       <c r="I21" t="str">
         <f t="shared" si="1"/>
         <v>30OCTEDA0304ACPMARRM_00001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>01NOVEDA0204DRRCMARRV_00001</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1238,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A3AD8B-A67B-4149-8F8C-48C0D9068BFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="D3:I3"/>
   <sheetViews>

</xml_diff>